<commit_message>
add formula explanation for deltaW
</commit_message>
<xml_diff>
--- a/pertemuan-14-28juni2023/tugas/jaringan-syaraf-tiruan-model-hebb/Model-Hebb.xlsx
+++ b/pertemuan-14-28juni2023/tugas/jaringan-syaraf-tiruan-model-hebb/Model-Hebb.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GIGABYTE-B550\Documents\kecerdasan-buatan-program\pertemuan-14\tugas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GIGABYTE-B550\Documents\kecerdasan-buatan-program\pertemuan-14-28juni2023\tugas\jaringan-syaraf-tiruan-model-hebb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B45C4D2C-0763-48AE-B59E-44940514E1C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B7E3EDB-BBA5-446C-9B45-B5406ECFE7AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{F2245345-A0E4-49C4-8BDF-B452C0ED2AAB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="63">
   <si>
     <t>Pola</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t xml:space="preserve">kesimpulan: dengan target 1 dan 2, pola rusak dapat dikenali oleh Model Hebb </t>
+  </si>
+  <si>
+    <t>Δw=xi.t</t>
   </si>
 </sst>
 </file>
@@ -322,18 +325,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -344,6 +335,18 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -661,8 +664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEF7CC9E-DD83-418C-9C00-CD60CE45CE37}">
   <dimension ref="A4:U74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="S59" sqref="S59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,37 +698,37 @@
       <c r="Q4" s="5"/>
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="10" t="s">
+      <c r="B5" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="K5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="14" t="s">
         <v>10</v>
       </c>
       <c r="N5" s="5" t="s">
@@ -736,17 +739,17 @@
       <c r="Q5" s="5"/>
     </row>
     <row r="6" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
       <c r="N6" s="5" t="s">
         <v>41</v>
       </c>
@@ -761,17 +764,17 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
       <c r="N7" s="5" t="s">
         <v>45</v>
       </c>
@@ -786,34 +789,34 @@
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="13">
-        <v>-1</v>
-      </c>
-      <c r="D8" s="13">
-        <v>-1</v>
-      </c>
-      <c r="E8" s="13">
-        <v>-1</v>
-      </c>
-      <c r="F8" s="13">
-        <v>1</v>
-      </c>
-      <c r="G8" s="13">
-        <v>-1</v>
-      </c>
-      <c r="H8" s="13">
-        <v>1</v>
-      </c>
-      <c r="I8" s="13">
-        <v>1</v>
-      </c>
-      <c r="J8" s="13">
-        <v>-1</v>
-      </c>
-      <c r="K8" s="13">
+      <c r="B8" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="9">
+        <v>-1</v>
+      </c>
+      <c r="D8" s="9">
+        <v>-1</v>
+      </c>
+      <c r="E8" s="9">
+        <v>-1</v>
+      </c>
+      <c r="F8" s="9">
+        <v>1</v>
+      </c>
+      <c r="G8" s="9">
+        <v>-1</v>
+      </c>
+      <c r="H8" s="9">
+        <v>1</v>
+      </c>
+      <c r="I8" s="9">
+        <v>1</v>
+      </c>
+      <c r="J8" s="9">
+        <v>-1</v>
+      </c>
+      <c r="K8" s="9">
         <v>1</v>
       </c>
       <c r="L8" s="4">
@@ -824,34 +827,34 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="14">
-        <v>-1</v>
-      </c>
-      <c r="D9" s="14">
-        <v>1</v>
-      </c>
-      <c r="E9" s="14">
-        <v>-1</v>
-      </c>
-      <c r="F9" s="14">
-        <v>-1</v>
-      </c>
-      <c r="G9" s="14">
-        <v>1</v>
-      </c>
-      <c r="H9" s="14">
-        <v>-1</v>
-      </c>
-      <c r="I9" s="14">
-        <v>-1</v>
-      </c>
-      <c r="J9" s="14">
-        <v>-1</v>
-      </c>
-      <c r="K9" s="14">
+      <c r="C9" s="10">
+        <v>-1</v>
+      </c>
+      <c r="D9" s="10">
+        <v>1</v>
+      </c>
+      <c r="E9" s="10">
+        <v>-1</v>
+      </c>
+      <c r="F9" s="10">
+        <v>-1</v>
+      </c>
+      <c r="G9" s="10">
+        <v>1</v>
+      </c>
+      <c r="H9" s="10">
+        <v>-1</v>
+      </c>
+      <c r="I9" s="10">
+        <v>-1</v>
+      </c>
+      <c r="J9" s="10">
+        <v>-1</v>
+      </c>
+      <c r="K9" s="10">
         <v>-1</v>
       </c>
       <c r="L9" s="4">
@@ -861,65 +864,70 @@
         <v>51</v>
       </c>
     </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="N10" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
     <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="10" t="s">
+      <c r="A13" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="I13" s="10" t="s">
+      <c r="I13" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="J13" s="10" t="s">
+      <c r="J13" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="K13" s="10" t="s">
+      <c r="K13" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="L13" s="10" t="s">
+      <c r="L13" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="10"/>
-      <c r="R13" s="10"/>
-      <c r="S13" s="10"/>
-      <c r="T13" s="10"/>
-      <c r="U13" s="10"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14"/>
+      <c r="S13" s="14"/>
+      <c r="T13" s="14"/>
+      <c r="U13" s="14"/>
     </row>
     <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
       <c r="L14" s="7" t="s">
         <v>19</v>
       </c>
@@ -952,7 +960,7 @@
       </c>
     </row>
     <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
+      <c r="A15" s="15"/>
       <c r="B15" s="3" t="s">
         <v>37</v>
       </c>
@@ -1018,43 +1026,43 @@
       <c r="A16" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="15">
+      <c r="B16" s="11">
         <f t="shared" ref="B16:J16" si="0">C8*$L$8</f>
         <v>-1</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="11">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="11">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="E16" s="15">
+      <c r="E16" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F16" s="11">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G16" s="15">
+      <c r="G16" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H16" s="15">
+      <c r="H16" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I16" s="15">
+      <c r="I16" s="11">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="J16" s="15">
+      <c r="J16" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K16" s="15">
+      <c r="K16" s="11">
         <f>$L$8</f>
         <v>1</v>
       </c>
@@ -1103,43 +1111,43 @@
       <c r="A17" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="16">
+      <c r="B17" s="12">
         <f t="shared" ref="B17:J17" si="2">C9*$L$9</f>
         <v>1</v>
       </c>
-      <c r="C17" s="16">
+      <c r="C17" s="12">
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="12">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E17" s="16">
+      <c r="E17" s="12">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="F17" s="16">
+      <c r="F17" s="12">
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-      <c r="G17" s="16">
+      <c r="G17" s="12">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="H17" s="16">
+      <c r="H17" s="12">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="I17" s="16">
+      <c r="I17" s="12">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="J17" s="16">
+      <c r="J17" s="12">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="K17" s="16">
+      <c r="K17" s="12">
         <f>$L$9</f>
         <v>-1</v>
       </c>
@@ -1185,35 +1193,35 @@
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="9" t="s">
+      <c r="A19" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="17" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="12"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="17"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="12"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="17"/>
     </row>
     <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
@@ -1263,34 +1271,34 @@
       <c r="D29" s="5"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B30" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C30" s="9" t="s">
+      <c r="B30" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D30" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E30" s="9" t="s">
+      <c r="E30" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F30" s="9" t="s">
+      <c r="F30" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G30" s="9" t="s">
+      <c r="G30" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="H30" s="9" t="s">
+      <c r="H30" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="I30" s="9" t="s">
+      <c r="I30" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="J30" s="9" t="s">
+      <c r="J30" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="K30" s="9" t="s">
+      <c r="K30" s="15" t="s">
         <v>9</v>
       </c>
       <c r="L30" t="s">
@@ -1298,16 +1306,16 @@
       </c>
     </row>
     <row r="31" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
       <c r="L31" s="8" t="s">
         <v>53</v>
       </c>
@@ -1403,64 +1411,64 @@
       <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B37" s="10" t="s">
+      <c r="A37" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C37" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="D37" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E37" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F37" s="10" t="s">
+      <c r="F37" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G37" s="10" t="s">
+      <c r="G37" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="H37" s="10" t="s">
+      <c r="H37" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="I37" s="10" t="s">
+      <c r="I37" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="J37" s="10" t="s">
+      <c r="J37" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="K37" s="10" t="s">
+      <c r="K37" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="L37" s="10" t="s">
+      <c r="L37" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="M37" s="10"/>
-      <c r="N37" s="10"/>
-      <c r="O37" s="10"/>
-      <c r="P37" s="10"/>
-      <c r="Q37" s="10"/>
-      <c r="R37" s="10"/>
-      <c r="S37" s="10"/>
-      <c r="T37" s="10"/>
-      <c r="U37" s="10"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="14"/>
+      <c r="P37" s="14"/>
+      <c r="Q37" s="14"/>
+      <c r="R37" s="14"/>
+      <c r="S37" s="14"/>
+      <c r="T37" s="14"/>
+      <c r="U37" s="14"/>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38" s="9"/>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="10"/>
-      <c r="K38" s="10"/>
+      <c r="A38" s="15"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
       <c r="L38" s="7" t="s">
         <v>19</v>
       </c>
@@ -1493,7 +1501,7 @@
       </c>
     </row>
     <row r="39" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="9"/>
+      <c r="A39" s="15"/>
       <c r="B39" s="3" t="s">
         <v>37</v>
       </c>
@@ -1731,35 +1739,35 @@
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A45" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B45" s="9" t="s">
+      <c r="A45" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="9" t="s">
+      <c r="C45" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D45" s="9" t="s">
+      <c r="D45" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E45" s="12" t="s">
+      <c r="E45" s="17" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="9"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="12"/>
+      <c r="A46" s="15"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="17"/>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A47" s="9"/>
-      <c r="B47" s="9"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="12"/>
+      <c r="A47" s="15"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="17"/>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
@@ -1814,64 +1822,64 @@
       <c r="D56" s="5"/>
     </row>
     <row r="57" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B57" s="10" t="s">
+      <c r="A57" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C57" s="10" t="s">
+      <c r="C57" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D57" s="10" t="s">
+      <c r="D57" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E57" s="10" t="s">
+      <c r="E57" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F57" s="10" t="s">
+      <c r="F57" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G57" s="10" t="s">
+      <c r="G57" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="H57" s="10" t="s">
+      <c r="H57" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="I57" s="10" t="s">
+      <c r="I57" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="J57" s="10" t="s">
+      <c r="J57" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="K57" s="10" t="s">
+      <c r="K57" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="L57" s="10" t="s">
+      <c r="L57" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="M57" s="10"/>
-      <c r="N57" s="10"/>
-      <c r="O57" s="10"/>
-      <c r="P57" s="10"/>
-      <c r="Q57" s="10"/>
-      <c r="R57" s="10"/>
-      <c r="S57" s="10"/>
-      <c r="T57" s="10"/>
-      <c r="U57" s="10"/>
+      <c r="M57" s="14"/>
+      <c r="N57" s="14"/>
+      <c r="O57" s="14"/>
+      <c r="P57" s="14"/>
+      <c r="Q57" s="14"/>
+      <c r="R57" s="14"/>
+      <c r="S57" s="14"/>
+      <c r="T57" s="14"/>
+      <c r="U57" s="14"/>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A58" s="9"/>
-      <c r="B58" s="10"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
-      <c r="E58" s="10"/>
-      <c r="F58" s="10"/>
-      <c r="G58" s="10"/>
-      <c r="H58" s="10"/>
-      <c r="I58" s="10"/>
-      <c r="J58" s="10"/>
-      <c r="K58" s="10"/>
+      <c r="A58" s="15"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="14"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="14"/>
+      <c r="J58" s="14"/>
+      <c r="K58" s="14"/>
       <c r="L58" s="7" t="s">
         <v>19</v>
       </c>
@@ -1904,7 +1912,7 @@
       </c>
     </row>
     <row r="59" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="9"/>
+      <c r="A59" s="15"/>
       <c r="B59" s="3" t="s">
         <v>37</v>
       </c>
@@ -2142,35 +2150,35 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B66" s="9" t="s">
+      <c r="A66" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B66" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C66" s="9" t="s">
+      <c r="C66" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D66" s="9" t="s">
+      <c r="D66" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E66" s="12" t="s">
+      <c r="E66" s="17" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="9"/>
-      <c r="B67" s="9"/>
-      <c r="C67" s="11"/>
-      <c r="D67" s="9"/>
-      <c r="E67" s="12"/>
+      <c r="A67" s="15"/>
+      <c r="B67" s="15"/>
+      <c r="C67" s="16"/>
+      <c r="D67" s="15"/>
+      <c r="E67" s="17"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="9"/>
-      <c r="B68" s="9"/>
-      <c r="C68" s="11"/>
-      <c r="D68" s="9"/>
-      <c r="E68" s="12"/>
+      <c r="A68" s="15"/>
+      <c r="B68" s="15"/>
+      <c r="C68" s="16"/>
+      <c r="D68" s="15"/>
+      <c r="E68" s="17"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
@@ -2219,18 +2227,50 @@
     </row>
   </sheetData>
   <mergeCells count="72">
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="H57:H58"/>
+    <mergeCell ref="I57:I58"/>
+    <mergeCell ref="J57:J58"/>
+    <mergeCell ref="K57:K58"/>
+    <mergeCell ref="L57:U57"/>
+    <mergeCell ref="B66:B68"/>
+    <mergeCell ref="C66:C68"/>
+    <mergeCell ref="D66:D68"/>
+    <mergeCell ref="E66:E68"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="G57:G58"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="E45:E47"/>
+    <mergeCell ref="D45:D47"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="I37:I38"/>
+    <mergeCell ref="J37:J38"/>
+    <mergeCell ref="K37:K38"/>
+    <mergeCell ref="L37:U37"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
     <mergeCell ref="I5:I7"/>
     <mergeCell ref="J5:J7"/>
     <mergeCell ref="K5:K7"/>
@@ -2247,50 +2287,18 @@
     <mergeCell ref="H5:H7"/>
     <mergeCell ref="L13:U13"/>
     <mergeCell ref="B13:B14"/>
-    <mergeCell ref="I37:I38"/>
-    <mergeCell ref="J37:J38"/>
-    <mergeCell ref="K37:K38"/>
-    <mergeCell ref="L37:U37"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="J30:J31"/>
-    <mergeCell ref="K30:K31"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="E45:E47"/>
-    <mergeCell ref="D45:D47"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="J57:J58"/>
-    <mergeCell ref="K57:K58"/>
-    <mergeCell ref="L57:U57"/>
-    <mergeCell ref="B66:B68"/>
-    <mergeCell ref="C66:C68"/>
-    <mergeCell ref="D66:D68"/>
-    <mergeCell ref="E66:E68"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="F57:F58"/>
-    <mergeCell ref="G57:G58"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="A66:A68"/>
-    <mergeCell ref="H57:H58"/>
-    <mergeCell ref="I57:I58"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>